<commit_message>
Update automatico via Actualizar 05-12-2020 15-48-05
</commit_message>
<xml_diff>
--- a/datacovidhn/ALIMENTACION_HN.xlsx
+++ b/datacovidhn/ALIMENTACION_HN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="8_{2E7B08DD-615A-4A26-9C8E-D4330F5D4097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B4EEF238-8C36-4433-9CFC-A6B55954CEA6}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="8_{2E7B08DD-615A-4A26-9C8E-D4330F5D4097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{86A3301F-9801-4054-ABCA-91DCD86CF704}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALIMENTACION" sheetId="1" r:id="rId1"/>
@@ -2259,9 +2259,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V255"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2420,10 +2420,10 @@
         <v>34</v>
       </c>
       <c r="U2" s="2">
-        <v>15.736700000000001</v>
+        <v>15.7857</v>
       </c>
       <c r="V2" s="2">
-        <v>-86.853399999999993</v>
+        <v>-86.793499999999995</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
@@ -2488,10 +2488,10 @@
         <v>39</v>
       </c>
       <c r="U3" s="2">
-        <v>15.7456</v>
+        <v>15.783799999999999</v>
       </c>
       <c r="V3" s="2">
-        <v>-86.851699999999994</v>
+        <v>-87.448300000000003</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
@@ -2556,10 +2556,10 @@
         <v>40</v>
       </c>
       <c r="U4" s="2">
-        <v>15.745900000000001</v>
+        <v>15.7843</v>
       </c>
       <c r="V4" s="2">
-        <v>-86.838700000000003</v>
+        <v>-87.449399999999997</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -2624,10 +2624,10 @@
         <v>41</v>
       </c>
       <c r="U5" s="2">
-        <v>15.765599999999999</v>
+        <v>15.784700000000001</v>
       </c>
       <c r="V5" s="2">
-        <v>-86.805999999999997</v>
+        <v>-87.450100000000006</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
@@ -2692,10 +2692,10 @@
         <v>48</v>
       </c>
       <c r="U6" s="2">
-        <v>15.7684</v>
+        <v>14.597899999999999</v>
       </c>
       <c r="V6" s="2">
-        <v>-86.802099999999996</v>
+        <v>-87.831299999999999</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
@@ -2760,10 +2760,10 @@
         <v>55</v>
       </c>
       <c r="U7" s="2">
-        <v>15.7684</v>
+        <v>15.425800000000001</v>
       </c>
       <c r="V7" s="2">
-        <v>-86.801900000000003</v>
+        <v>-88.013900000000007</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
@@ -2828,10 +2828,10 @@
         <v>56</v>
       </c>
       <c r="U8" s="2">
-        <v>15.7685</v>
+        <v>15.514099999999999</v>
       </c>
       <c r="V8" s="2">
-        <v>-86.8018</v>
+        <v>-88.012699999999995</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
@@ -2896,10 +2896,10 @@
         <v>57</v>
       </c>
       <c r="U9" s="2">
-        <v>15.769500000000001</v>
+        <v>15.514699999999999</v>
       </c>
       <c r="V9" s="2">
-        <v>-86.790700000000001</v>
+        <v>-88.013000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
@@ -2964,10 +2964,10 @@
         <v>58</v>
       </c>
       <c r="U10" s="2">
-        <v>15.7699</v>
+        <v>15.5158</v>
       </c>
       <c r="V10" s="2">
-        <v>-86.797399999999996</v>
+        <v>-88.017300000000006</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -3032,10 +3032,10 @@
         <v>59</v>
       </c>
       <c r="U11" s="2">
-        <v>15.770099999999999</v>
+        <v>15.5327</v>
       </c>
       <c r="V11" s="2">
-        <v>-86.793300000000002</v>
+        <v>-88.027799999999999</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
@@ -3100,10 +3100,10 @@
         <v>66</v>
       </c>
       <c r="U12" s="2">
-        <v>15.7705</v>
+        <v>14.1061</v>
       </c>
       <c r="V12" s="2">
-        <v>-86.790800000000004</v>
+        <v>-87.155199999999994</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
@@ -3168,10 +3168,10 @@
         <v>71</v>
       </c>
       <c r="U13" s="2">
-        <v>15.7707</v>
+        <v>14.5419</v>
       </c>
       <c r="V13" s="2">
-        <v>-86.792199999999994</v>
+        <v>-86.827299999999994</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
@@ -3236,10 +3236,10 @@
         <v>79</v>
       </c>
       <c r="U14" s="2">
-        <v>15.7707</v>
+        <v>15.536099999999999</v>
       </c>
       <c r="V14" s="2">
-        <v>-86.799300000000002</v>
+        <v>-87.653099999999995</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
@@ -3304,10 +3304,10 @@
         <v>80</v>
       </c>
       <c r="U15" s="2">
-        <v>15.7712</v>
+        <v>15.7707</v>
       </c>
       <c r="V15" s="2">
-        <v>-86.790599999999998</v>
+        <v>-86.799300000000002</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
@@ -3440,10 +3440,10 @@
         <v>82</v>
       </c>
       <c r="U17" s="2">
-        <v>15.7728</v>
+        <v>15.7828</v>
       </c>
       <c r="V17" s="2">
-        <v>-86.793000000000006</v>
+        <v>-86.790700000000001</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
@@ -3508,10 +3508,10 @@
         <v>85</v>
       </c>
       <c r="U18" s="2">
-        <v>15.773</v>
+        <v>15.7714</v>
       </c>
       <c r="V18" s="2">
-        <v>-86.793000000000006</v>
+        <v>-86.801199999999994</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
@@ -3576,10 +3576,10 @@
         <v>86</v>
       </c>
       <c r="U19" s="2">
-        <v>15.773199999999999</v>
+        <v>15.774900000000001</v>
       </c>
       <c r="V19" s="2">
-        <v>-86.792500000000004</v>
+        <v>-86.803700000000006</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
@@ -3644,10 +3644,10 @@
         <v>87</v>
       </c>
       <c r="U20" s="2">
-        <v>15.7735</v>
+        <v>15.7629</v>
       </c>
       <c r="V20" s="2">
-        <v>-86.791200000000003</v>
+        <v>-87.477099999999993</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
@@ -3712,10 +3712,10 @@
         <v>88</v>
       </c>
       <c r="U21" s="2">
-        <v>15.774100000000001</v>
+        <v>15.763199999999999</v>
       </c>
       <c r="V21" s="2">
-        <v>-86.790499999999994</v>
+        <v>-87.476100000000002</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
@@ -3780,10 +3780,10 @@
         <v>58</v>
       </c>
       <c r="U22" s="2">
-        <v>15.775399999999999</v>
+        <v>15.765000000000001</v>
       </c>
       <c r="V22" s="2">
-        <v>-86.790499999999994</v>
+        <v>-87.480400000000003</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
@@ -3848,10 +3848,10 @@
         <v>89</v>
       </c>
       <c r="U23" s="2">
-        <v>15.7761</v>
+        <v>15.7738</v>
       </c>
       <c r="V23" s="2">
-        <v>-86.8001</v>
+        <v>-87.475300000000004</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
@@ -3916,10 +3916,10 @@
         <v>87</v>
       </c>
       <c r="U24" s="2">
-        <v>15.7761</v>
+        <v>15.774699999999999</v>
       </c>
       <c r="V24" s="2">
-        <v>-86.8001</v>
+        <v>-87.473600000000005</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
@@ -3984,10 +3984,10 @@
         <v>90</v>
       </c>
       <c r="U25" s="2">
-        <v>15.7761</v>
+        <v>15.7803</v>
       </c>
       <c r="V25" s="2">
-        <v>-86.8</v>
+        <v>-87.456800000000001</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
@@ -4052,10 +4052,10 @@
         <v>91</v>
       </c>
       <c r="U26" s="2">
-        <v>15.776199999999999</v>
+        <v>15.7841</v>
       </c>
       <c r="V26" s="2">
-        <v>-86.8</v>
+        <v>-87.450699999999998</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
@@ -4120,10 +4120,10 @@
         <v>92</v>
       </c>
       <c r="U27" s="2">
-        <v>15.7765</v>
+        <v>15.7841</v>
       </c>
       <c r="V27" s="2">
-        <v>-86.799099999999996</v>
+        <v>-87.449700000000007</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
@@ -4188,10 +4188,10 @@
         <v>93</v>
       </c>
       <c r="U28" s="2">
-        <v>15.7766</v>
+        <v>15.7841</v>
       </c>
       <c r="V28" s="2">
-        <v>-86.790999999999997</v>
+        <v>-87.450900000000004</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
@@ -4256,10 +4256,10 @@
         <v>94</v>
       </c>
       <c r="U29" s="2">
-        <v>15.7768</v>
+        <v>15.7842</v>
       </c>
       <c r="V29" s="2">
-        <v>-86.787400000000005</v>
+        <v>-87.449399999999997</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
@@ -4324,10 +4324,10 @@
         <v>87</v>
       </c>
       <c r="U30" s="2">
-        <v>15.776899999999999</v>
+        <v>15.7844</v>
       </c>
       <c r="V30" s="2">
-        <v>-86.768199999999993</v>
+        <v>-87.450999999999993</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
@@ -4392,10 +4392,10 @@
         <v>95</v>
       </c>
       <c r="U31" s="2">
-        <v>15.776999999999999</v>
+        <v>15.7845</v>
       </c>
       <c r="V31" s="2">
-        <v>-86.790499999999994</v>
+        <v>-87.450599999999994</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
@@ -4460,10 +4460,10 @@
         <v>96</v>
       </c>
       <c r="U32" s="2">
-        <v>15.777100000000001</v>
+        <v>15.7852</v>
       </c>
       <c r="V32" s="2">
-        <v>-86.790800000000004</v>
+        <v>-87.450400000000002</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
@@ -4528,10 +4528,10 @@
         <v>97</v>
       </c>
       <c r="U33" s="2">
-        <v>15.777100000000001</v>
+        <v>15.785299999999999</v>
       </c>
       <c r="V33" s="2">
-        <v>-86.787599999999998</v>
+        <v>-87.450400000000002</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
@@ -4596,10 +4596,10 @@
         <v>87</v>
       </c>
       <c r="U34" s="2">
-        <v>15.7773</v>
+        <v>15.7591</v>
       </c>
       <c r="V34" s="2">
-        <v>-86.787400000000005</v>
+        <v>-87.49</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
@@ -4664,10 +4664,10 @@
         <v>102</v>
       </c>
       <c r="U35" s="2">
-        <v>15.7776</v>
+        <v>15.5754</v>
       </c>
       <c r="V35" s="2">
-        <v>-86.787599999999998</v>
+        <v>-87.616299999999995</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
@@ -4732,10 +4732,10 @@
         <v>87</v>
       </c>
       <c r="U36" s="2">
-        <v>15.7782</v>
+        <v>15.7072</v>
       </c>
       <c r="V36" s="2">
-        <v>-86.786000000000001</v>
+        <v>-87.584199999999996</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
@@ -4800,10 +4800,10 @@
         <v>87</v>
       </c>
       <c r="U37" s="2">
-        <v>15.7782</v>
+        <v>15.6684</v>
       </c>
       <c r="V37" s="2">
-        <v>-86.786000000000001</v>
+        <v>-87.602000000000004</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
@@ -4868,10 +4868,10 @@
         <v>107</v>
       </c>
       <c r="U38" s="2">
-        <v>15.778499999999999</v>
+        <v>15.6686</v>
       </c>
       <c r="V38" s="2">
-        <v>-86.7881</v>
+        <v>-87.601799999999997</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
@@ -4936,10 +4936,10 @@
         <v>112</v>
       </c>
       <c r="U39" s="2">
-        <v>15.7791</v>
+        <v>15.682399999999999</v>
       </c>
       <c r="V39" s="2">
-        <v>-86.788499999999999</v>
+        <v>-87.332099999999997</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
@@ -5004,10 +5004,10 @@
         <v>113</v>
       </c>
       <c r="U40" s="2">
-        <v>15.779199999999999</v>
+        <v>15.682600000000001</v>
       </c>
       <c r="V40" s="2">
-        <v>-86.788899999999998</v>
+        <v>-87.331999999999994</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
@@ -5072,10 +5072,10 @@
         <v>117</v>
       </c>
       <c r="U41" s="2">
-        <v>15.779199999999999</v>
+        <v>14.424099999999999</v>
       </c>
       <c r="V41" s="2">
-        <v>-86.788899999999998</v>
+        <v>-87.632900000000006</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
@@ -5140,10 +5140,10 @@
         <v>118</v>
       </c>
       <c r="U42" s="2">
-        <v>15.779400000000001</v>
+        <v>14.4582</v>
       </c>
       <c r="V42" s="2">
-        <v>-86.801000000000002</v>
+        <v>-87.640699999999995</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.3">
@@ -5208,10 +5208,10 @@
         <v>123</v>
       </c>
       <c r="U43" s="2">
-        <v>15.779500000000001</v>
+        <v>14.2614</v>
       </c>
       <c r="V43" s="2">
-        <v>-86.773099999999999</v>
+        <v>-87.613399999999999</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.3">
@@ -5276,10 +5276,10 @@
         <v>124</v>
       </c>
       <c r="U44" s="2">
-        <v>15.779500000000001</v>
+        <v>14.591799999999999</v>
       </c>
       <c r="V44" s="2">
-        <v>-86.788799999999995</v>
+        <v>-87.834299999999999</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.3">
@@ -5344,10 +5344,10 @@
         <v>87</v>
       </c>
       <c r="U45" s="2">
-        <v>15.779500000000001</v>
+        <v>15.4755</v>
       </c>
       <c r="V45" s="2">
-        <v>-86.800899999999999</v>
+        <v>-87.991</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.3">
@@ -5412,10 +5412,10 @@
         <v>87</v>
       </c>
       <c r="U46" s="2">
-        <v>15.7796</v>
+        <v>15.4756</v>
       </c>
       <c r="V46" s="2">
-        <v>-86.789100000000005</v>
+        <v>-87.990399999999994</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.3">
@@ -5480,10 +5480,10 @@
         <v>125</v>
       </c>
       <c r="U47" s="2">
-        <v>15.7797</v>
+        <v>15.4757</v>
       </c>
       <c r="V47" s="2">
-        <v>-86.790099999999995</v>
+        <v>-87.990300000000005</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.3">
@@ -5548,10 +5548,10 @@
         <v>87</v>
       </c>
       <c r="U48" s="2">
-        <v>15.7798</v>
+        <v>15.4764</v>
       </c>
       <c r="V48" s="2">
-        <v>-86.789199999999994</v>
+        <v>-87.99</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.3">
@@ -5616,10 +5616,10 @@
         <v>87</v>
       </c>
       <c r="U49" s="2">
-        <v>15.7799</v>
+        <v>15.477</v>
       </c>
       <c r="V49" s="2">
-        <v>-86.801000000000002</v>
+        <v>-87.989800000000002</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.3">
@@ -5684,10 +5684,10 @@
         <v>87</v>
       </c>
       <c r="U50" s="2">
-        <v>15.780099999999999</v>
+        <v>15.4808</v>
       </c>
       <c r="V50" s="2">
-        <v>-86.801599999999993</v>
+        <v>-88.014600000000002</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.3">
@@ -5752,10 +5752,10 @@
         <v>87</v>
       </c>
       <c r="U51" s="2">
-        <v>15.780200000000001</v>
+        <v>15.4918</v>
       </c>
       <c r="V51" s="2">
-        <v>-86.792699999999996</v>
+        <v>-87.998999999999995</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.3">
@@ -5820,10 +5820,10 @@
         <v>126</v>
       </c>
       <c r="U52" s="2">
-        <v>15.7803</v>
+        <v>15.4922</v>
       </c>
       <c r="V52" s="2">
-        <v>-86.773099999999999</v>
+        <v>-88.002300000000005</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.3">
@@ -5888,10 +5888,10 @@
         <v>127</v>
       </c>
       <c r="U53" s="2">
-        <v>15.7806</v>
+        <v>15.4941</v>
       </c>
       <c r="V53" s="2">
-        <v>-86.792599999999993</v>
+        <v>-88.022499999999994</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.3">
@@ -5956,10 +5956,10 @@
         <v>128</v>
       </c>
       <c r="U54" s="2">
-        <v>15.7806</v>
+        <v>15.5009</v>
       </c>
       <c r="V54" s="2">
-        <v>-86.789699999999996</v>
+        <v>-88.029200000000003</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.3">
@@ -6024,10 +6024,10 @@
         <v>129</v>
       </c>
       <c r="U55" s="2">
-        <v>15.7807</v>
+        <v>15.5044</v>
       </c>
       <c r="V55" s="2">
-        <v>-86.792500000000004</v>
+        <v>-88.016800000000003</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.3">
@@ -6092,10 +6092,10 @@
         <v>130</v>
       </c>
       <c r="U56" s="2">
-        <v>15.780799999999999</v>
+        <v>15.504899999999999</v>
       </c>
       <c r="V56" s="2">
-        <v>-86.790999999999997</v>
+        <v>-88.044399999999996</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.3">
@@ -6160,10 +6160,10 @@
         <v>87</v>
       </c>
       <c r="U57" s="2">
-        <v>15.780900000000001</v>
+        <v>15.505599999999999</v>
       </c>
       <c r="V57" s="2">
-        <v>-86.79</v>
+        <v>-88.005799999999994</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.3">
@@ -6228,10 +6228,10 @@
         <v>131</v>
       </c>
       <c r="U58" s="2">
-        <v>15.7812</v>
+        <v>15.513199999999999</v>
       </c>
       <c r="V58" s="2">
-        <v>-86.790899999999993</v>
+        <v>-88.038300000000007</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.3">
@@ -6296,10 +6296,10 @@
         <v>87</v>
       </c>
       <c r="U59" s="2">
-        <v>15.7813</v>
+        <v>15.5444</v>
       </c>
       <c r="V59" s="2">
-        <v>-86.791300000000007</v>
+        <v>-88.003100000000003</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.3">
@@ -6364,10 +6364,10 @@
         <v>136</v>
       </c>
       <c r="U60" s="2">
-        <v>15.781499999999999</v>
+        <v>15.8452</v>
       </c>
       <c r="V60" s="2">
-        <v>-86.790499999999994</v>
+        <v>-87.944699999999997</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.3">
@@ -6432,10 +6432,10 @@
         <v>137</v>
       </c>
       <c r="U61" s="2">
-        <v>15.781499999999999</v>
+        <v>15.845700000000001</v>
       </c>
       <c r="V61" s="2">
-        <v>-86.790400000000005</v>
+        <v>-87.939899999999994</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.3">
@@ -6500,10 +6500,10 @@
         <v>143</v>
       </c>
       <c r="U62" s="2">
-        <v>15.781499999999999</v>
+        <v>15.0579</v>
       </c>
       <c r="V62" s="2">
-        <v>-86.790300000000002</v>
+        <v>-87.983500000000006</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.3">
@@ -6568,10 +6568,10 @@
         <v>149</v>
       </c>
       <c r="U63" s="2">
-        <v>15.781599999999999</v>
+        <v>14.907500000000001</v>
       </c>
       <c r="V63" s="2">
-        <v>-86.790999999999997</v>
+        <v>-87.936899999999994</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.3">
@@ -6636,10 +6636,10 @@
         <v>87</v>
       </c>
       <c r="U64" s="2">
-        <v>15.781700000000001</v>
+        <v>14.0182</v>
       </c>
       <c r="V64" s="2">
-        <v>-86.790499999999994</v>
+        <v>-86.670199999999994</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.3">
@@ -6704,10 +6704,10 @@
         <v>87</v>
       </c>
       <c r="U65" s="2">
-        <v>15.7822</v>
+        <v>14.0396</v>
       </c>
       <c r="V65" s="2">
-        <v>-86.790400000000005</v>
+        <v>-87.206100000000006</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.3">
@@ -6772,10 +6772,10 @@
         <v>87</v>
       </c>
       <c r="U66" s="2">
-        <v>15.782299999999999</v>
+        <v>14.0402</v>
       </c>
       <c r="V66" s="2">
-        <v>-86.790400000000005</v>
+        <v>-87.203900000000004</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.3">
@@ -6840,10 +6840,10 @@
         <v>156</v>
       </c>
       <c r="U67" s="2">
-        <v>15.782400000000001</v>
+        <v>14.053599999999999</v>
       </c>
       <c r="V67" s="2">
-        <v>-86.790499999999994</v>
+        <v>-87.233199999999997</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
@@ -6908,10 +6908,10 @@
         <v>157</v>
       </c>
       <c r="U68" s="2">
-        <v>15.7828</v>
+        <v>14.060499999999999</v>
       </c>
       <c r="V68" s="2">
-        <v>-86.790700000000001</v>
+        <v>-87.226799999999997</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.3">
@@ -6976,10 +6976,10 @@
         <v>158</v>
       </c>
       <c r="U69" s="2">
-        <v>15.7829</v>
+        <v>14.0686</v>
       </c>
       <c r="V69" s="2">
-        <v>-86.790999999999997</v>
+        <v>-87.218000000000004</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.3">
@@ -7044,10 +7044,10 @@
         <v>159</v>
       </c>
       <c r="U70" s="2">
-        <v>15.7829</v>
+        <v>14.072800000000001</v>
       </c>
       <c r="V70" s="2">
-        <v>-86.790999999999997</v>
+        <v>-87.176199999999994</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.3">
@@ -7112,10 +7112,10 @@
         <v>160</v>
       </c>
       <c r="U71" s="2">
-        <v>15.7829</v>
+        <v>14.0732</v>
       </c>
       <c r="V71" s="2">
-        <v>-86.790800000000004</v>
+        <v>-87.170699999999997</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.3">
@@ -7180,10 +7180,10 @@
         <v>161</v>
       </c>
       <c r="U72" s="2">
-        <v>15.7829</v>
+        <v>14.074400000000001</v>
       </c>
       <c r="V72" s="2">
-        <v>-86.790999999999997</v>
+        <v>-87.168099999999995</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.3">
@@ -7248,10 +7248,10 @@
         <v>162</v>
       </c>
       <c r="U73" s="2">
-        <v>15.7834</v>
+        <v>14.08</v>
       </c>
       <c r="V73" s="2">
-        <v>-86.792400000000001</v>
+        <v>-87.189700000000002</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.3">
@@ -7316,10 +7316,10 @@
         <v>163</v>
       </c>
       <c r="U74" s="2">
-        <v>15.7835</v>
+        <v>14.0815</v>
       </c>
       <c r="V74" s="2">
-        <v>-86.790499999999994</v>
+        <v>-87.202799999999996</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.3">
@@ -7384,10 +7384,10 @@
         <v>157</v>
       </c>
       <c r="U75" s="2">
-        <v>15.7836</v>
+        <v>14.0824</v>
       </c>
       <c r="V75" s="2">
-        <v>-86.792500000000004</v>
+        <v>-87.166799999999995</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.3">
@@ -7452,10 +7452,10 @@
         <v>164</v>
       </c>
       <c r="U76" s="2">
-        <v>15.7836</v>
+        <v>14.0848</v>
       </c>
       <c r="V76" s="2">
-        <v>-86.791200000000003</v>
+        <v>-87.180899999999994</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.3">
@@ -7520,10 +7520,10 @@
         <v>165</v>
       </c>
       <c r="U77" s="2">
-        <v>15.7837</v>
+        <v>14.091799999999999</v>
       </c>
       <c r="V77" s="2">
-        <v>-86.792500000000004</v>
+        <v>-87.213200000000001</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.3">
@@ -7588,10 +7588,10 @@
         <v>166</v>
       </c>
       <c r="U78" s="2">
-        <v>15.783899999999999</v>
+        <v>14.093999999999999</v>
       </c>
       <c r="V78" s="2">
-        <v>-86.791399999999996</v>
+        <v>-87.1708</v>
       </c>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.3">
@@ -7656,10 +7656,10 @@
         <v>167</v>
       </c>
       <c r="U79" s="2">
-        <v>15.7842</v>
+        <v>14.094900000000001</v>
       </c>
       <c r="V79" s="2">
-        <v>-86.792500000000004</v>
+        <v>-87.181299999999993</v>
       </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.3">
@@ -7724,10 +7724,10 @@
         <v>168</v>
       </c>
       <c r="U80" s="2">
-        <v>15.7843</v>
+        <v>14.099299999999999</v>
       </c>
       <c r="V80" s="2">
-        <v>-86.794300000000007</v>
+        <v>-87.162400000000005</v>
       </c>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.3">
@@ -7792,10 +7792,10 @@
         <v>169</v>
       </c>
       <c r="U81" s="2">
-        <v>15.7844</v>
+        <v>14.0997</v>
       </c>
       <c r="V81" s="2">
-        <v>-86.791899999999998</v>
+        <v>-87.188299999999998</v>
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.3">
@@ -7860,10 +7860,10 @@
         <v>170</v>
       </c>
       <c r="U82" s="2">
-        <v>15.7845</v>
+        <v>14.0998</v>
       </c>
       <c r="V82" s="2">
-        <v>-86.791899999999998</v>
+        <v>-87.181299999999993</v>
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.3">
@@ -7928,10 +7928,10 @@
         <v>157</v>
       </c>
       <c r="U83" s="2">
-        <v>15.7845</v>
+        <v>14.0999</v>
       </c>
       <c r="V83" s="2">
-        <v>-86.792699999999996</v>
+        <v>-87.186099999999996</v>
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.3">
@@ -7996,10 +7996,10 @@
         <v>170</v>
       </c>
       <c r="U84" s="2">
-        <v>15.784599999999999</v>
+        <v>14.1008</v>
       </c>
       <c r="V84" s="2">
-        <v>-86.792000000000002</v>
+        <v>-87.180300000000003</v>
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.3">
@@ -8064,10 +8064,10 @@
         <v>171</v>
       </c>
       <c r="U85" s="2">
-        <v>15.784700000000001</v>
+        <v>14.1014</v>
       </c>
       <c r="V85" s="2">
-        <v>-86.793700000000001</v>
+        <v>-87.207899999999995</v>
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.3">
@@ -8132,10 +8132,10 @@
         <v>172</v>
       </c>
       <c r="U86" s="2">
-        <v>15.784800000000001</v>
+        <v>14.102399999999999</v>
       </c>
       <c r="V86" s="2">
-        <v>-86.792900000000003</v>
+        <v>-87.185199999999995</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.3">
@@ -8200,10 +8200,10 @@
         <v>87</v>
       </c>
       <c r="U87" s="2">
-        <v>15.784800000000001</v>
+        <v>14.1027</v>
       </c>
       <c r="V87" s="2">
-        <v>-86.790899999999993</v>
+        <v>-87.184399999999997</v>
       </c>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.3">
@@ -8268,10 +8268,10 @@
         <v>157</v>
       </c>
       <c r="U88" s="2">
-        <v>15.784800000000001</v>
+        <v>14.104100000000001</v>
       </c>
       <c r="V88" s="2">
-        <v>-86.792400000000001</v>
+        <v>-87.193600000000004</v>
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.3">
@@ -8336,10 +8336,10 @@
         <v>173</v>
       </c>
       <c r="U89" s="2">
-        <v>15.7849</v>
+        <v>14.104900000000001</v>
       </c>
       <c r="V89" s="2">
-        <v>-86.791899999999998</v>
+        <v>-87.154700000000005</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.3">
@@ -8404,10 +8404,10 @@
         <v>174</v>
       </c>
       <c r="U90" s="2">
-        <v>15.7849</v>
+        <v>14.1058</v>
       </c>
       <c r="V90" s="2">
-        <v>-86.793099999999995</v>
+        <v>-87.154899999999998</v>
       </c>
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.3">
@@ -8472,10 +8472,10 @@
         <v>175</v>
       </c>
       <c r="U91" s="2">
-        <v>15.7849</v>
+        <v>14.1059</v>
       </c>
       <c r="V91" s="2">
-        <v>-86.792100000000005</v>
+        <v>-87.155199999999994</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.3">
@@ -8540,10 +8540,10 @@
         <v>176</v>
       </c>
       <c r="U92" s="2">
-        <v>15.785</v>
+        <v>14.1068</v>
       </c>
       <c r="V92" s="2">
-        <v>-86.792000000000002</v>
+        <v>-87.155799999999999</v>
       </c>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.3">
@@ -8608,10 +8608,10 @@
         <v>177</v>
       </c>
       <c r="U93" s="2">
-        <v>15.7851</v>
+        <v>14.107100000000001</v>
       </c>
       <c r="V93" s="2">
-        <v>-86.791700000000006</v>
+        <v>-87.222399999999993</v>
       </c>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.3">
@@ -8676,10 +8676,10 @@
         <v>178</v>
       </c>
       <c r="U94" s="2">
-        <v>15.7852</v>
+        <v>14.1076</v>
       </c>
       <c r="V94" s="2">
-        <v>-86.792100000000005</v>
+        <v>-87.156499999999994</v>
       </c>
     </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.3">
@@ -8744,10 +8744,10 @@
         <v>179</v>
       </c>
       <c r="U95" s="2">
-        <v>15.7852</v>
+        <v>14.1082</v>
       </c>
       <c r="V95" s="2">
-        <v>-86.787899999999993</v>
+        <v>-87.156599999999997</v>
       </c>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.3">
@@ -8812,10 +8812,10 @@
         <v>180</v>
       </c>
       <c r="U96" s="2">
-        <v>15.7852</v>
+        <v>14.1084</v>
       </c>
       <c r="V96" s="2">
-        <v>-86.793400000000005</v>
+        <v>-87.157200000000003</v>
       </c>
     </row>
     <row r="97" spans="1:22" x14ac:dyDescent="0.3">
@@ -8880,10 +8880,10 @@
         <v>181</v>
       </c>
       <c r="U97" s="2">
-        <v>15.7852</v>
+        <v>14.108700000000001</v>
       </c>
       <c r="V97" s="2">
-        <v>-86.792100000000005</v>
+        <v>-87.156599999999997</v>
       </c>
     </row>
     <row r="98" spans="1:22" x14ac:dyDescent="0.3">
@@ -8948,10 +8948,10 @@
         <v>181</v>
       </c>
       <c r="U98" s="2">
-        <v>15.785299999999999</v>
+        <v>14.109400000000001</v>
       </c>
       <c r="V98" s="2">
-        <v>-86.791300000000007</v>
+        <v>-87.156400000000005</v>
       </c>
     </row>
     <row r="99" spans="1:22" x14ac:dyDescent="0.3">
@@ -9016,10 +9016,10 @@
         <v>182</v>
       </c>
       <c r="U99" s="2">
-        <v>15.785299999999999</v>
+        <v>14.109500000000001</v>
       </c>
       <c r="V99" s="2">
-        <v>-86.788200000000003</v>
+        <v>-87.155900000000003</v>
       </c>
     </row>
     <row r="100" spans="1:22" x14ac:dyDescent="0.3">
@@ -9084,10 +9084,10 @@
         <v>183</v>
       </c>
       <c r="U100" s="2">
-        <v>15.785299999999999</v>
+        <v>14.11</v>
       </c>
       <c r="V100" s="2">
-        <v>-86.791700000000006</v>
+        <v>-87.156300000000002</v>
       </c>
     </row>
     <row r="101" spans="1:22" x14ac:dyDescent="0.3">
@@ -9152,10 +9152,10 @@
         <v>157</v>
       </c>
       <c r="U101" s="2">
-        <v>15.785399999999999</v>
+        <v>14.113799999999999</v>
       </c>
       <c r="V101" s="2">
-        <v>-86.793400000000005</v>
+        <v>-87.193700000000007</v>
       </c>
     </row>
     <row r="102" spans="1:22" x14ac:dyDescent="0.3">
@@ -9220,10 +9220,10 @@
         <v>184</v>
       </c>
       <c r="U102" s="2">
-        <v>15.785399999999999</v>
+        <v>14.116300000000001</v>
       </c>
       <c r="V102" s="2">
-        <v>-86.790999999999997</v>
+        <v>-87.209599999999995</v>
       </c>
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.3">
@@ -9288,10 +9288,10 @@
         <v>189</v>
       </c>
       <c r="U103" s="2">
-        <v>15.785500000000001</v>
+        <v>14.162800000000001</v>
       </c>
       <c r="V103" s="2">
-        <v>-86.792500000000004</v>
+        <v>-87.0441</v>
       </c>
     </row>
     <row r="104" spans="1:22" x14ac:dyDescent="0.3">
@@ -9356,10 +9356,10 @@
         <v>197</v>
       </c>
       <c r="U104" s="2">
-        <v>15.785600000000001</v>
+        <v>16.3157</v>
       </c>
       <c r="V104" s="2">
-        <v>-86.792299999999997</v>
+        <v>-86.5398</v>
       </c>
     </row>
     <row r="105" spans="1:22" x14ac:dyDescent="0.3">
@@ -9424,10 +9424,10 @@
         <v>198</v>
       </c>
       <c r="U105" s="2">
-        <v>15.785600000000001</v>
+        <v>16.3169</v>
       </c>
       <c r="V105" s="2">
-        <v>-86.792500000000004</v>
+        <v>-86.538799999999995</v>
       </c>
     </row>
     <row r="106" spans="1:22" x14ac:dyDescent="0.3">
@@ -9492,10 +9492,10 @@
         <v>199</v>
       </c>
       <c r="U106" s="2">
-        <v>15.7857</v>
+        <v>16.317299999999999</v>
       </c>
       <c r="V106" s="2">
-        <v>-86.793499999999995</v>
+        <v>-86.537599999999998</v>
       </c>
     </row>
     <row r="107" spans="1:22" x14ac:dyDescent="0.3">
@@ -9560,10 +9560,10 @@
         <v>200</v>
       </c>
       <c r="U107" s="2">
-        <v>15.7857</v>
+        <v>16.332599999999999</v>
       </c>
       <c r="V107" s="2">
-        <v>-86.792599999999993</v>
+        <v>-86.539699999999996</v>
       </c>
     </row>
     <row r="108" spans="1:22" x14ac:dyDescent="0.3">
@@ -9628,10 +9628,10 @@
         <v>203</v>
       </c>
       <c r="U108" s="2">
-        <v>15.7858</v>
+        <v>16.305</v>
       </c>
       <c r="V108" s="2">
-        <v>-86.792400000000001</v>
+        <v>-86.5565</v>
       </c>
     </row>
     <row r="109" spans="1:22" x14ac:dyDescent="0.3">
@@ -9696,10 +9696,10 @@
         <v>87</v>
       </c>
       <c r="U109" s="2">
-        <v>15.7859</v>
+        <v>16.312100000000001</v>
       </c>
       <c r="V109" s="2">
-        <v>-86.792500000000004</v>
+        <v>-86.581100000000006</v>
       </c>
     </row>
     <row r="110" spans="1:22" x14ac:dyDescent="0.3">
@@ -9764,10 +9764,10 @@
         <v>87</v>
       </c>
       <c r="U110" s="2">
-        <v>15.786099999999999</v>
+        <v>16.3307</v>
       </c>
       <c r="V110" s="2">
-        <v>-86.7928</v>
+        <v>-86.567300000000003</v>
       </c>
     </row>
     <row r="111" spans="1:22" x14ac:dyDescent="0.3">
@@ -9832,10 +9832,10 @@
         <v>208</v>
       </c>
       <c r="U111" s="2">
-        <v>15.786099999999999</v>
+        <v>16.278099999999998</v>
       </c>
       <c r="V111" s="2">
-        <v>-86.792599999999993</v>
+        <v>-86.5989</v>
       </c>
     </row>
     <row r="112" spans="1:22" x14ac:dyDescent="0.3">
@@ -9900,10 +9900,10 @@
         <v>209</v>
       </c>
       <c r="U112" s="2">
-        <v>15.7864</v>
+        <v>16.3048</v>
       </c>
       <c r="V112" s="2">
-        <v>-86.7941</v>
+        <v>-86.593800000000002</v>
       </c>
     </row>
     <row r="113" spans="1:22" x14ac:dyDescent="0.3">
@@ -9968,10 +9968,10 @@
         <v>210</v>
       </c>
       <c r="U113" s="2">
-        <v>15.7864</v>
+        <v>16.305700000000002</v>
       </c>
       <c r="V113" s="2">
-        <v>-86.792900000000003</v>
+        <v>-86.592699999999994</v>
       </c>
     </row>
     <row r="114" spans="1:22" x14ac:dyDescent="0.3">
@@ -10036,10 +10036,10 @@
         <v>216</v>
       </c>
       <c r="U114" s="2">
-        <v>15.7866</v>
+        <v>16.063800000000001</v>
       </c>
       <c r="V114" s="2">
-        <v>-86.793000000000006</v>
+        <v>-86.967399999999998</v>
       </c>
     </row>
     <row r="115" spans="1:22" x14ac:dyDescent="0.3">
@@ -10104,10 +10104,10 @@
         <v>217</v>
       </c>
       <c r="U115" s="2">
-        <v>15.786799999999999</v>
+        <v>16.063800000000001</v>
       </c>
       <c r="V115" s="2">
-        <v>-86.790599999999998</v>
+        <v>-86.967100000000002</v>
       </c>
     </row>
     <row r="116" spans="1:22" x14ac:dyDescent="0.3">
@@ -10172,10 +10172,10 @@
         <v>218</v>
       </c>
       <c r="U116" s="2">
-        <v>15.786899999999999</v>
+        <v>16.0641</v>
       </c>
       <c r="V116" s="2">
-        <v>-86.793099999999995</v>
+        <v>-86.965000000000003</v>
       </c>
     </row>
     <row r="117" spans="1:22" x14ac:dyDescent="0.3">
@@ -10240,10 +10240,10 @@
         <v>219</v>
       </c>
       <c r="U117" s="2">
-        <v>15.786899999999999</v>
+        <v>16.0642</v>
       </c>
       <c r="V117" s="2">
-        <v>-86.793099999999995</v>
+        <v>-86.965800000000002</v>
       </c>
     </row>
     <row r="118" spans="1:22" x14ac:dyDescent="0.3">
@@ -10308,10 +10308,10 @@
         <v>220</v>
       </c>
       <c r="U118" s="2">
-        <v>15.787000000000001</v>
+        <v>16.0944</v>
       </c>
       <c r="V118" s="2">
-        <v>-86.793099999999995</v>
+        <v>-86.892399999999995</v>
       </c>
     </row>
     <row r="119" spans="1:22" x14ac:dyDescent="0.3">
@@ -10376,10 +10376,10 @@
         <v>221</v>
       </c>
       <c r="U119" s="2">
-        <v>15.787100000000001</v>
+        <v>16.0961</v>
       </c>
       <c r="V119" s="2">
-        <v>-86.793400000000005</v>
+        <v>-86.894000000000005</v>
       </c>
     </row>
     <row r="120" spans="1:22" x14ac:dyDescent="0.3">
@@ -10444,10 +10444,10 @@
         <v>157</v>
       </c>
       <c r="U120" s="2">
-        <v>15.7872</v>
+        <v>16.102</v>
       </c>
       <c r="V120" s="2">
-        <v>-86.792500000000004</v>
+        <v>-86.894000000000005</v>
       </c>
     </row>
     <row r="121" spans="1:22" x14ac:dyDescent="0.3">
@@ -10512,10 +10512,10 @@
         <v>228</v>
       </c>
       <c r="U121" s="2">
-        <v>15.787699999999999</v>
+        <v>14.5891</v>
       </c>
       <c r="V121" s="2">
-        <v>-86.793700000000001</v>
+        <v>-88.582700000000003</v>
       </c>
     </row>
     <row r="122" spans="1:22" x14ac:dyDescent="0.3">
@@ -10580,10 +10580,10 @@
         <v>229</v>
       </c>
       <c r="U122" s="2">
-        <v>15.7883</v>
+        <v>14.590400000000001</v>
       </c>
       <c r="V122" s="2">
-        <v>-86.782700000000006</v>
+        <v>-88.584000000000003</v>
       </c>
     </row>
     <row r="123" spans="1:22" x14ac:dyDescent="0.3">
@@ -10648,10 +10648,10 @@
         <v>230</v>
       </c>
       <c r="U123" s="2">
-        <v>15.789400000000001</v>
+        <v>14.594900000000001</v>
       </c>
       <c r="V123" s="2">
-        <v>-86.792699999999996</v>
+        <v>-88.581699999999998</v>
       </c>
     </row>
     <row r="124" spans="1:22" x14ac:dyDescent="0.3">
@@ -10716,10 +10716,10 @@
         <v>238</v>
       </c>
       <c r="U124" s="2">
-        <v>15.7896</v>
+        <v>13.268700000000001</v>
       </c>
       <c r="V124" s="2">
-        <v>-86.792500000000004</v>
+        <v>-87.657600000000002</v>
       </c>
     </row>
     <row r="125" spans="1:22" x14ac:dyDescent="0.3">
@@ -10784,10 +10784,10 @@
         <v>87</v>
       </c>
       <c r="U125" s="2">
-        <v>15.7898</v>
+        <v>15.5343</v>
       </c>
       <c r="V125" s="2">
-        <v>-86.792100000000005</v>
+        <v>-87.653300000000002</v>
       </c>
     </row>
     <row r="126" spans="1:22" x14ac:dyDescent="0.3">
@@ -10852,10 +10852,10 @@
         <v>87</v>
       </c>
       <c r="U126" s="2">
-        <v>15.7902</v>
+        <v>15.5425</v>
       </c>
       <c r="V126" s="2">
-        <v>-86.792299999999997</v>
+        <v>-87.6524</v>
       </c>
     </row>
     <row r="127" spans="1:22" x14ac:dyDescent="0.3">
@@ -10920,10 +10920,10 @@
         <v>241</v>
       </c>
       <c r="U127" s="2">
-        <v>15.7906</v>
+        <v>15.549799999999999</v>
       </c>
       <c r="V127" s="2">
-        <v>-86.784499999999994</v>
+        <v>-87.651600000000002</v>
       </c>
     </row>
     <row r="128" spans="1:22" x14ac:dyDescent="0.3">
@@ -10988,10 +10988,10 @@
         <v>87</v>
       </c>
       <c r="U128" s="2">
-        <v>15.790800000000001</v>
+        <v>15.550800000000001</v>
       </c>
       <c r="V128" s="2">
-        <v>-86.790300000000002</v>
+        <v>-87.651399999999995</v>
       </c>
     </row>
     <row r="129" spans="1:22" x14ac:dyDescent="0.3">
@@ -11056,10 +11056,10 @@
         <v>87</v>
       </c>
       <c r="U129" s="2">
-        <v>15.790900000000001</v>
+        <v>15.552</v>
       </c>
       <c r="V129" s="2">
-        <v>-86.790300000000002</v>
+        <v>-87.651300000000006</v>
       </c>
     </row>
     <row r="130" spans="1:22" x14ac:dyDescent="0.3">
@@ -11124,10 +11124,10 @@
         <v>246</v>
       </c>
       <c r="U130" s="2">
-        <v>15.790900000000001</v>
+        <v>15.401400000000001</v>
       </c>
       <c r="V130" s="2">
-        <v>-86.790099999999995</v>
+        <v>-87.806600000000003</v>
       </c>
     </row>
     <row r="131" spans="1:22" x14ac:dyDescent="0.3">
@@ -11192,10 +11192,10 @@
         <v>247</v>
       </c>
       <c r="U131" s="2">
-        <v>15.791</v>
+        <v>15.402200000000001</v>
       </c>
       <c r="V131" s="2">
-        <v>-86.79</v>
+        <v>-87.802899999999994</v>
       </c>
     </row>
     <row r="132" spans="1:22" x14ac:dyDescent="0.3">
@@ -11260,10 +11260,10 @@
         <v>250</v>
       </c>
       <c r="U132" s="2">
-        <v>15.791399999999999</v>
+        <v>15.4876</v>
       </c>
       <c r="V132" s="2">
-        <v>-86.789500000000004</v>
+        <v>-87.758799999999994</v>
       </c>
     </row>
     <row r="133" spans="1:22" x14ac:dyDescent="0.3">
@@ -11328,10 +11328,10 @@
         <v>251</v>
       </c>
       <c r="U133" s="2">
-        <v>15.792299999999999</v>
+        <v>15.488</v>
       </c>
       <c r="V133" s="2">
-        <v>-86.788399999999996</v>
+        <v>-87.758899999999997</v>
       </c>
     </row>
     <row r="134" spans="1:22" x14ac:dyDescent="0.3">
@@ -11396,10 +11396,10 @@
         <v>252</v>
       </c>
       <c r="U134" s="2">
-        <v>15.792899999999999</v>
+        <v>14.0586</v>
       </c>
       <c r="V134" s="2">
-        <v>-86.764499999999998</v>
+        <v>-87.190100000000001</v>
       </c>
     </row>
     <row r="135" spans="1:22" x14ac:dyDescent="0.3">
@@ -11464,10 +11464,10 @@
         <v>253</v>
       </c>
       <c r="U135" s="2">
-        <v>15.7934</v>
+        <v>14.0589</v>
       </c>
       <c r="V135" s="2">
-        <v>-86.7624</v>
+        <v>-87.189400000000006</v>
       </c>
     </row>
     <row r="136" spans="1:22" x14ac:dyDescent="0.3">
@@ -11532,10 +11532,10 @@
         <v>254</v>
       </c>
       <c r="U136" s="2">
-        <v>15.794</v>
+        <v>14.058999999999999</v>
       </c>
       <c r="V136" s="2">
-        <v>-86.762100000000004</v>
+        <v>-87.189499999999995</v>
       </c>
     </row>
     <row r="137" spans="1:22" x14ac:dyDescent="0.3">
@@ -11600,10 +11600,10 @@
         <v>255</v>
       </c>
       <c r="U137" s="2">
-        <v>15.794600000000001</v>
+        <v>14.5405</v>
       </c>
       <c r="V137" s="2">
-        <v>-86.785600000000002</v>
+        <v>-86.829899999999995</v>
       </c>
     </row>
     <row r="138" spans="1:22" x14ac:dyDescent="0.3">
@@ -11668,10 +11668,10 @@
         <v>256</v>
       </c>
       <c r="U138" s="2">
-        <v>15.7951</v>
+        <v>14.5405</v>
       </c>
       <c r="V138" s="2">
-        <v>-86.783799999999999</v>
+        <v>-86.827500000000001</v>
       </c>
     </row>
     <row r="139" spans="1:22" x14ac:dyDescent="0.3">
@@ -11736,10 +11736,10 @@
         <v>257</v>
       </c>
       <c r="U139" s="2">
-        <v>15.7516</v>
+        <v>14.5444</v>
       </c>
       <c r="V139" s="2">
-        <v>-86.872100000000003</v>
+        <v>-86.829899999999995</v>
       </c>
     </row>
     <row r="140" spans="1:22" x14ac:dyDescent="0.3">
@@ -11804,10 +11804,10 @@
         <v>263</v>
       </c>
       <c r="U140" s="2">
-        <v>15.7532</v>
+        <v>14.438499999999999</v>
       </c>
       <c r="V140" s="2">
-        <v>-86.870900000000006</v>
+        <v>-89.183300000000003</v>
       </c>
     </row>
     <row r="141" spans="1:22" x14ac:dyDescent="0.3">
@@ -11872,10 +11872,10 @@
         <v>264</v>
       </c>
       <c r="U141" s="2">
-        <v>15.753399999999999</v>
+        <v>15.7735</v>
       </c>
       <c r="V141" s="2">
-        <v>-86.871099999999998</v>
+        <v>-86.791200000000003</v>
       </c>
     </row>
     <row r="142" spans="1:22" x14ac:dyDescent="0.3">
@@ -11940,10 +11940,10 @@
         <v>265</v>
       </c>
       <c r="U142" s="2">
-        <v>15.7547</v>
+        <v>15.777100000000001</v>
       </c>
       <c r="V142" s="2">
-        <v>-86.872699999999995</v>
+        <v>-86.787599999999998</v>
       </c>
     </row>
     <row r="143" spans="1:22" x14ac:dyDescent="0.3">
@@ -12008,10 +12008,10 @@
         <v>266</v>
       </c>
       <c r="U143" s="2">
-        <v>15.754799999999999</v>
+        <v>15.7829</v>
       </c>
       <c r="V143" s="2">
-        <v>-86.870199999999997</v>
+        <v>-87.450199999999995</v>
       </c>
     </row>
     <row r="144" spans="1:22" x14ac:dyDescent="0.3">
@@ -12076,10 +12076,10 @@
         <v>267</v>
       </c>
       <c r="U144" s="2">
-        <v>15.7552</v>
+        <v>15.7829</v>
       </c>
       <c r="V144" s="2">
-        <v>-86.869100000000003</v>
+        <v>-87.4512</v>
       </c>
     </row>
     <row r="145" spans="1:22" x14ac:dyDescent="0.3">
@@ -12144,10 +12144,10 @@
         <v>268</v>
       </c>
       <c r="U145" s="2">
-        <v>15.756600000000001</v>
+        <v>14.454000000000001</v>
       </c>
       <c r="V145" s="2">
-        <v>-86.872500000000002</v>
+        <v>-87.638900000000007</v>
       </c>
     </row>
     <row r="146" spans="1:22" x14ac:dyDescent="0.3">
@@ -12212,10 +12212,10 @@
         <v>268</v>
       </c>
       <c r="U146" s="2">
-        <v>15.7567</v>
+        <v>14.4597</v>
       </c>
       <c r="V146" s="2">
-        <v>-86.871399999999994</v>
+        <v>-87.6447</v>
       </c>
     </row>
     <row r="147" spans="1:22" x14ac:dyDescent="0.3">
@@ -12280,10 +12280,10 @@
         <v>269</v>
       </c>
       <c r="U147" s="2">
-        <v>15.7567</v>
+        <v>14.462300000000001</v>
       </c>
       <c r="V147" s="2">
-        <v>-86.869500000000002</v>
+        <v>-87.645600000000002</v>
       </c>
     </row>
     <row r="148" spans="1:22" x14ac:dyDescent="0.3">
@@ -12348,10 +12348,10 @@
         <v>270</v>
       </c>
       <c r="U148" s="2">
-        <v>15.7568</v>
+        <v>14.590199999999999</v>
       </c>
       <c r="V148" s="2">
-        <v>-86.871499999999997</v>
+        <v>-87.833200000000005</v>
       </c>
     </row>
     <row r="149" spans="1:22" x14ac:dyDescent="0.3">
@@ -12416,10 +12416,10 @@
         <v>271</v>
       </c>
       <c r="U149" s="2">
-        <v>15.757</v>
+        <v>15.486000000000001</v>
       </c>
       <c r="V149" s="2">
-        <v>-86.874399999999994</v>
+        <v>-88.014600000000002</v>
       </c>
     </row>
     <row r="150" spans="1:22" x14ac:dyDescent="0.3">
@@ -12484,10 +12484,10 @@
         <v>272</v>
       </c>
       <c r="U150" s="2">
-        <v>15.7575</v>
+        <v>15.493499999999999</v>
       </c>
       <c r="V150" s="2">
-        <v>-86.875399999999999</v>
+        <v>-87.984300000000005</v>
       </c>
     </row>
     <row r="151" spans="1:22" x14ac:dyDescent="0.3">
@@ -12552,10 +12552,10 @@
         <v>273</v>
       </c>
       <c r="U151" s="2">
-        <v>15.7577</v>
+        <v>15.498200000000001</v>
       </c>
       <c r="V151" s="2">
-        <v>-86.866299999999995</v>
+        <v>-88.046199999999999</v>
       </c>
     </row>
     <row r="152" spans="1:22" x14ac:dyDescent="0.3">
@@ -12620,10 +12620,10 @@
         <v>274</v>
       </c>
       <c r="U152" s="2">
-        <v>15.758100000000001</v>
+        <v>15.5021</v>
       </c>
       <c r="V152" s="2">
-        <v>-86.870699999999999</v>
+        <v>-88.036600000000007</v>
       </c>
     </row>
     <row r="153" spans="1:22" x14ac:dyDescent="0.3">
@@ -12688,10 +12688,10 @@
         <v>275</v>
       </c>
       <c r="U153" s="2">
-        <v>15.7583</v>
+        <v>15.507</v>
       </c>
       <c r="V153" s="2">
-        <v>-86.870900000000006</v>
+        <v>-88.027000000000001</v>
       </c>
     </row>
     <row r="154" spans="1:22" x14ac:dyDescent="0.3">
@@ -12756,10 +12756,10 @@
         <v>276</v>
       </c>
       <c r="U154" s="2">
-        <v>15.759600000000001</v>
+        <v>15.5124</v>
       </c>
       <c r="V154" s="2">
-        <v>-86.868300000000005</v>
+        <v>-88.036699999999996</v>
       </c>
     </row>
     <row r="155" spans="1:22" x14ac:dyDescent="0.3">
@@ -12824,10 +12824,10 @@
         <v>281</v>
       </c>
       <c r="U155" s="2">
-        <v>15.7597</v>
+        <v>15.565899999999999</v>
       </c>
       <c r="V155" s="2">
-        <v>-86.877200000000002</v>
+        <v>-87.959500000000006</v>
       </c>
     </row>
     <row r="156" spans="1:22" x14ac:dyDescent="0.3">
@@ -12892,10 +12892,10 @@
         <v>282</v>
       </c>
       <c r="U156" s="2">
-        <v>15.7601</v>
+        <v>15.6111</v>
       </c>
       <c r="V156" s="2">
-        <v>-86.876000000000005</v>
+        <v>-87.956100000000006</v>
       </c>
     </row>
     <row r="157" spans="1:22" x14ac:dyDescent="0.3">
@@ -12960,10 +12960,10 @@
         <v>284</v>
       </c>
       <c r="U157" s="2">
-        <v>15.7615</v>
+        <v>15.845499999999999</v>
       </c>
       <c r="V157" s="2">
-        <v>-86.875600000000006</v>
+        <v>-87.942499999999995</v>
       </c>
     </row>
     <row r="158" spans="1:22" x14ac:dyDescent="0.3">
@@ -13028,10 +13028,10 @@
         <v>285</v>
       </c>
       <c r="U158" s="2">
-        <v>15.7616</v>
+        <v>14.045199999999999</v>
       </c>
       <c r="V158" s="2">
-        <v>-86.869600000000005</v>
+        <v>-87.211500000000001</v>
       </c>
     </row>
     <row r="159" spans="1:22" x14ac:dyDescent="0.3">
@@ -13096,10 +13096,10 @@
         <v>285</v>
       </c>
       <c r="U159" s="2">
-        <v>15.7616</v>
+        <v>14.0458</v>
       </c>
       <c r="V159" s="2">
-        <v>-86.876400000000004</v>
+        <v>-87.2119</v>
       </c>
     </row>
     <row r="160" spans="1:22" x14ac:dyDescent="0.3">
@@ -13164,10 +13164,10 @@
         <v>286</v>
       </c>
       <c r="U160" s="2">
-        <v>15.7804</v>
+        <v>14.058999999999999</v>
       </c>
       <c r="V160" s="2">
-        <v>-86.680999999999997</v>
+        <v>-87.220600000000005</v>
       </c>
     </row>
     <row r="161" spans="1:22" x14ac:dyDescent="0.3">
@@ -13232,10 +13232,10 @@
         <v>287</v>
       </c>
       <c r="U161" s="2">
-        <v>15.787100000000001</v>
+        <v>14.060600000000001</v>
       </c>
       <c r="V161" s="2">
-        <v>-86.680800000000005</v>
+        <v>-87.220500000000001</v>
       </c>
     </row>
     <row r="162" spans="1:22" x14ac:dyDescent="0.3">
@@ -13300,10 +13300,10 @@
         <v>285</v>
       </c>
       <c r="U162" s="2">
-        <v>15.7631</v>
+        <v>14.065200000000001</v>
       </c>
       <c r="V162" s="2">
-        <v>-86.818899999999999</v>
+        <v>-87.1785</v>
       </c>
     </row>
     <row r="163" spans="1:22" x14ac:dyDescent="0.3">
@@ -13368,10 +13368,10 @@
         <v>285</v>
       </c>
       <c r="U163" s="2">
-        <v>15.7714</v>
+        <v>14.068</v>
       </c>
       <c r="V163" s="2">
-        <v>-86.801199999999994</v>
+        <v>-87.182699999999997</v>
       </c>
     </row>
     <row r="164" spans="1:22" x14ac:dyDescent="0.3">
@@ -13436,10 +13436,10 @@
         <v>288</v>
       </c>
       <c r="U164" s="2">
-        <v>15.774900000000001</v>
+        <v>14.069000000000001</v>
       </c>
       <c r="V164" s="2">
-        <v>-86.803700000000006</v>
+        <v>-87.184799999999996</v>
       </c>
     </row>
     <row r="165" spans="1:22" x14ac:dyDescent="0.3">
@@ -13504,10 +13504,10 @@
         <v>285</v>
       </c>
       <c r="U165" s="2">
-        <v>15.774900000000001</v>
+        <v>14.076700000000001</v>
       </c>
       <c r="V165" s="2">
-        <v>-86.8048</v>
+        <v>-87.186000000000007</v>
       </c>
     </row>
     <row r="166" spans="1:22" x14ac:dyDescent="0.3">
@@ -13572,10 +13572,10 @@
         <v>289</v>
       </c>
       <c r="U166" s="2">
-        <v>15.7751</v>
+        <v>14.0768</v>
       </c>
       <c r="V166" s="2">
-        <v>-86.8035</v>
+        <v>-87.186000000000007</v>
       </c>
     </row>
     <row r="167" spans="1:22" x14ac:dyDescent="0.3">
@@ -13640,10 +13640,10 @@
         <v>285</v>
       </c>
       <c r="U167" s="2">
-        <v>15.775600000000001</v>
+        <v>14.0852</v>
       </c>
       <c r="V167" s="2">
-        <v>-86.802599999999998</v>
+        <v>-87.186899999999994</v>
       </c>
     </row>
     <row r="168" spans="1:22" x14ac:dyDescent="0.3">
@@ -13708,10 +13708,10 @@
         <v>290</v>
       </c>
       <c r="U168" s="2">
-        <v>15.7759</v>
+        <v>14.0969</v>
       </c>
       <c r="V168" s="2">
-        <v>-86.803799999999995</v>
+        <v>-87.221999999999994</v>
       </c>
     </row>
     <row r="169" spans="1:22" x14ac:dyDescent="0.3">
@@ -13776,10 +13776,10 @@
         <v>285</v>
       </c>
       <c r="U169" s="2">
-        <v>15.777200000000001</v>
+        <v>14.098699999999999</v>
       </c>
       <c r="V169" s="2">
-        <v>-86.801599999999993</v>
+        <v>-87.227099999999993</v>
       </c>
     </row>
     <row r="170" spans="1:22" x14ac:dyDescent="0.3">
@@ -13844,10 +13844,10 @@
         <v>291</v>
       </c>
       <c r="U170" s="2">
-        <v>15.777200000000001</v>
+        <v>14.1006</v>
       </c>
       <c r="V170" s="2">
-        <v>-86.801500000000004</v>
+        <v>-87.193799999999996</v>
       </c>
     </row>
     <row r="171" spans="1:22" x14ac:dyDescent="0.3">
@@ -13912,10 +13912,10 @@
         <v>287</v>
       </c>
       <c r="U171" s="2">
-        <v>15.7773</v>
+        <v>14.1006</v>
       </c>
       <c r="V171" s="2">
-        <v>-86.801599999999993</v>
+        <v>-87.193899999999999</v>
       </c>
     </row>
     <row r="172" spans="1:22" x14ac:dyDescent="0.3">
@@ -13980,10 +13980,10 @@
         <v>292</v>
       </c>
       <c r="U172" s="2">
-        <v>15.7774</v>
+        <v>14.101699999999999</v>
       </c>
       <c r="V172" s="2">
-        <v>-86.801299999999998</v>
+        <v>-87.186800000000005</v>
       </c>
     </row>
     <row r="173" spans="1:22" x14ac:dyDescent="0.3">
@@ -14048,10 +14048,10 @@
         <v>285</v>
       </c>
       <c r="U173" s="2">
-        <v>15.7776</v>
+        <v>14.1058</v>
       </c>
       <c r="V173" s="2">
-        <v>-86.801199999999994</v>
+        <v>-87.197400000000002</v>
       </c>
     </row>
     <row r="174" spans="1:22" x14ac:dyDescent="0.3">
@@ -14116,10 +14116,10 @@
         <v>293</v>
       </c>
       <c r="U174" s="2">
-        <v>15.781599999999999</v>
+        <v>14.555400000000001</v>
       </c>
       <c r="V174" s="2">
-        <v>-86.802800000000005</v>
+        <v>-86.827799999999996</v>
       </c>
     </row>
     <row r="175" spans="1:22" x14ac:dyDescent="0.3">
@@ -14184,10 +14184,10 @@
         <v>294</v>
       </c>
       <c r="U175" s="2">
-        <v>15.6366</v>
+        <v>16.3063</v>
       </c>
       <c r="V175" s="2">
-        <v>-86.651200000000003</v>
+        <v>-86.589200000000005</v>
       </c>
     </row>
     <row r="176" spans="1:22" x14ac:dyDescent="0.3">
@@ -14252,10 +14252,10 @@
         <v>301</v>
       </c>
       <c r="U176" s="2">
-        <v>15.701499999999999</v>
+        <v>14.1562</v>
       </c>
       <c r="V176" s="2">
-        <v>-86.72</v>
+        <v>-88.035899999999998</v>
       </c>
     </row>
     <row r="177" spans="1:22" x14ac:dyDescent="0.3">
@@ -14320,10 +14320,10 @@
         <v>302</v>
       </c>
       <c r="U177" s="2">
-        <v>15.726900000000001</v>
+        <v>14.587300000000001</v>
       </c>
       <c r="V177" s="2">
-        <v>-86.740700000000004</v>
+        <v>-88.583100000000002</v>
       </c>
     </row>
     <row r="178" spans="1:22" x14ac:dyDescent="0.3">
@@ -14388,10 +14388,10 @@
         <v>303</v>
       </c>
       <c r="U178" s="2">
-        <v>15.7827</v>
+        <v>14.436299999999999</v>
       </c>
       <c r="V178" s="2">
-        <v>-86.684799999999996</v>
+        <v>-89.182299999999998</v>
       </c>
     </row>
     <row r="179" spans="1:22" x14ac:dyDescent="0.3">
@@ -14456,10 +14456,10 @@
         <v>304</v>
       </c>
       <c r="U179" s="2">
-        <v>15.7874</v>
+        <v>15.396100000000001</v>
       </c>
       <c r="V179" s="2">
-        <v>-86.688199999999995</v>
+        <v>-87.802400000000006</v>
       </c>
     </row>
     <row r="180" spans="1:22" x14ac:dyDescent="0.3">
@@ -14524,10 +14524,10 @@
         <v>305</v>
       </c>
       <c r="U180" s="2">
-        <v>15.662000000000001</v>
+        <v>15.399699999999999</v>
       </c>
       <c r="V180" s="2">
-        <v>-86.694599999999994</v>
+        <v>-87.811000000000007</v>
       </c>
     </row>
     <row r="181" spans="1:22" x14ac:dyDescent="0.3">
@@ -14592,10 +14592,10 @@
         <v>306</v>
       </c>
       <c r="U181" s="2">
-        <v>15.786799999999999</v>
+        <v>15.402200000000001</v>
       </c>
       <c r="V181" s="2">
-        <v>-86.619600000000005</v>
+        <v>-87.806399999999996</v>
       </c>
     </row>
     <row r="182" spans="1:22" x14ac:dyDescent="0.3">
@@ -14660,10 +14660,10 @@
         <v>307</v>
       </c>
       <c r="U182" s="2">
-        <v>15.7875</v>
+        <v>15.4023</v>
       </c>
       <c r="V182" s="2">
-        <v>-86.619500000000002</v>
+        <v>-87.807199999999995</v>
       </c>
     </row>
     <row r="183" spans="1:22" x14ac:dyDescent="0.3">
@@ -14728,10 +14728,10 @@
         <v>308</v>
       </c>
       <c r="U183" s="2">
-        <v>15.7963</v>
+        <v>15.776899999999999</v>
       </c>
       <c r="V183" s="2">
-        <v>-86.621300000000005</v>
+        <v>-86.768199999999993</v>
       </c>
     </row>
     <row r="184" spans="1:22" x14ac:dyDescent="0.3">
@@ -14796,10 +14796,10 @@
         <v>309</v>
       </c>
       <c r="U184" s="2">
-        <v>15.7416</v>
+        <v>15.784700000000001</v>
       </c>
       <c r="V184" s="2">
-        <v>-86.873400000000004</v>
+        <v>-86.793700000000001</v>
       </c>
     </row>
     <row r="185" spans="1:22" x14ac:dyDescent="0.3">
@@ -14864,10 +14864,10 @@
         <v>310</v>
       </c>
       <c r="U185" s="2">
-        <v>15.743399999999999</v>
+        <v>15.7851</v>
       </c>
       <c r="V185" s="2">
-        <v>-87.174199999999999</v>
+        <v>-86.791700000000006</v>
       </c>
     </row>
     <row r="186" spans="1:22" x14ac:dyDescent="0.3">
@@ -14932,10 +14932,10 @@
         <v>308</v>
       </c>
       <c r="U186" s="2">
-        <v>15.5977</v>
+        <v>15.783200000000001</v>
       </c>
       <c r="V186" s="2">
-        <v>-87.221299999999999</v>
+        <v>-87.451099999999997</v>
       </c>
     </row>
     <row r="187" spans="1:22" x14ac:dyDescent="0.3">
@@ -15000,10 +15000,10 @@
         <v>311</v>
       </c>
       <c r="U187" s="2">
-        <v>15.598800000000001</v>
+        <v>14.591699999999999</v>
       </c>
       <c r="V187" s="2">
-        <v>-87.217699999999994</v>
+        <v>-87.834299999999999</v>
       </c>
     </row>
     <row r="188" spans="1:22" x14ac:dyDescent="0.3">
@@ -15068,10 +15068,10 @@
         <v>311</v>
       </c>
       <c r="U188" s="2">
-        <v>15.6204</v>
+        <v>14.591799999999999</v>
       </c>
       <c r="V188" s="2">
-        <v>-87.094099999999997</v>
+        <v>-87.834199999999996</v>
       </c>
     </row>
     <row r="189" spans="1:22" x14ac:dyDescent="0.3">
@@ -15136,10 +15136,10 @@
         <v>311</v>
       </c>
       <c r="U189" s="2">
-        <v>15.5983</v>
+        <v>14.591900000000001</v>
       </c>
       <c r="V189" s="2">
-        <v>-87.216200000000001</v>
+        <v>-87.834199999999996</v>
       </c>
     </row>
     <row r="190" spans="1:22" x14ac:dyDescent="0.3">
@@ -15204,10 +15204,10 @@
         <v>308</v>
       </c>
       <c r="U190" s="2">
-        <v>15.5985</v>
+        <v>14.765599999999999</v>
       </c>
       <c r="V190" s="2">
-        <v>-87.216200000000001</v>
+        <v>-88.774699999999996</v>
       </c>
     </row>
     <row r="191" spans="1:22" x14ac:dyDescent="0.3">
@@ -15272,10 +15272,10 @@
         <v>319</v>
       </c>
       <c r="U191" s="2">
-        <v>15.5985</v>
+        <v>14.766</v>
       </c>
       <c r="V191" s="2">
-        <v>-87.214200000000005</v>
+        <v>-88.777199999999993</v>
       </c>
     </row>
     <row r="192" spans="1:22" x14ac:dyDescent="0.3">
@@ -15340,10 +15340,10 @@
         <v>325</v>
       </c>
       <c r="U192" s="2">
-        <v>15.5985</v>
+        <v>14.8377</v>
       </c>
       <c r="V192" s="2">
-        <v>-87.213999999999999</v>
+        <v>-89.156499999999994</v>
       </c>
     </row>
     <row r="193" spans="1:22" x14ac:dyDescent="0.3">
@@ -15408,10 +15408,10 @@
         <v>308</v>
       </c>
       <c r="U193" s="2">
-        <v>15.598599999999999</v>
+        <v>14.8407</v>
       </c>
       <c r="V193" s="2">
-        <v>-87.212699999999998</v>
+        <v>-89.155100000000004</v>
       </c>
     </row>
     <row r="194" spans="1:22" x14ac:dyDescent="0.3">
@@ -15476,10 +15476,10 @@
         <v>326</v>
       </c>
       <c r="U194" s="2">
-        <v>15.598699999999999</v>
+        <v>15.4938</v>
       </c>
       <c r="V194" s="2">
-        <v>-87.215400000000002</v>
+        <v>-87.983800000000002</v>
       </c>
     </row>
     <row r="195" spans="1:22" x14ac:dyDescent="0.3">
@@ -15544,10 +15544,10 @@
         <v>311</v>
       </c>
       <c r="U195" s="2">
-        <v>15.598800000000001</v>
+        <v>15.4971</v>
       </c>
       <c r="V195" s="2">
-        <v>-87.211100000000002</v>
+        <v>-87.987799999999993</v>
       </c>
     </row>
     <row r="196" spans="1:22" x14ac:dyDescent="0.3">
@@ -15612,10 +15612,10 @@
         <v>311</v>
       </c>
       <c r="U196" s="2">
-        <v>15.5989</v>
+        <v>15.5052</v>
       </c>
       <c r="V196" s="2">
-        <v>-87.208799999999997</v>
+        <v>-88.012</v>
       </c>
     </row>
     <row r="197" spans="1:22" x14ac:dyDescent="0.3">
@@ -15680,10 +15680,10 @@
         <v>311</v>
       </c>
       <c r="U197" s="2">
-        <v>15.5989</v>
+        <v>15.519600000000001</v>
       </c>
       <c r="V197" s="2">
-        <v>-87.211399999999998</v>
+        <v>-88.024799999999999</v>
       </c>
     </row>
     <row r="198" spans="1:22" x14ac:dyDescent="0.3">
@@ -15748,10 +15748,10 @@
         <v>327</v>
       </c>
       <c r="U198" s="2">
-        <v>15.5989</v>
+        <v>15.527100000000001</v>
       </c>
       <c r="V198" s="2">
-        <v>-87.213899999999995</v>
+        <v>-88.034899999999993</v>
       </c>
     </row>
     <row r="199" spans="1:22" x14ac:dyDescent="0.3">
@@ -15816,10 +15816,10 @@
         <v>328</v>
       </c>
       <c r="U199" s="2">
-        <v>15.599</v>
+        <v>15.603999999999999</v>
       </c>
       <c r="V199" s="2">
-        <v>-87.208200000000005</v>
+        <v>-87.953900000000004</v>
       </c>
     </row>
     <row r="200" spans="1:22" x14ac:dyDescent="0.3">
@@ -15884,10 +15884,10 @@
         <v>329</v>
       </c>
       <c r="U200" s="2">
-        <v>15.599</v>
+        <v>15.611599999999999</v>
       </c>
       <c r="V200" s="2">
-        <v>-87.210800000000006</v>
+        <v>-87.9465</v>
       </c>
     </row>
     <row r="201" spans="1:22" x14ac:dyDescent="0.3">
@@ -15952,10 +15952,10 @@
         <v>326</v>
       </c>
       <c r="U201" s="2">
-        <v>15.5992</v>
+        <v>15.613099999999999</v>
       </c>
       <c r="V201" s="2">
-        <v>-87.212299999999999</v>
+        <v>-87.957300000000004</v>
       </c>
     </row>
     <row r="202" spans="1:22" x14ac:dyDescent="0.3">
@@ -16020,10 +16020,10 @@
         <v>319</v>
       </c>
       <c r="U202" s="2">
-        <v>15.599399999999999</v>
+        <v>15.66</v>
       </c>
       <c r="V202" s="2">
-        <v>-87.204800000000006</v>
+        <v>-88.1982</v>
       </c>
     </row>
     <row r="203" spans="1:22" x14ac:dyDescent="0.3">
@@ -16088,10 +16088,10 @@
         <v>328</v>
       </c>
       <c r="U203" s="2">
-        <v>15.599399999999999</v>
+        <v>15.8446</v>
       </c>
       <c r="V203" s="2">
-        <v>-87.206400000000002</v>
+        <v>-87.933800000000005</v>
       </c>
     </row>
     <row r="204" spans="1:22" x14ac:dyDescent="0.3">
@@ -16156,10 +16156,10 @@
         <v>308</v>
       </c>
       <c r="U204" s="2">
-        <v>15.599500000000001</v>
+        <v>15.845000000000001</v>
       </c>
       <c r="V204" s="2">
-        <v>-87.205500000000001</v>
+        <v>-87.945400000000006</v>
       </c>
     </row>
     <row r="205" spans="1:22" x14ac:dyDescent="0.3">
@@ -16224,10 +16224,10 @@
         <v>335</v>
       </c>
       <c r="U205" s="2">
-        <v>15.599600000000001</v>
+        <v>15.847099999999999</v>
       </c>
       <c r="V205" s="2">
-        <v>-87.199399999999997</v>
+        <v>-87.946700000000007</v>
       </c>
     </row>
     <row r="206" spans="1:22" x14ac:dyDescent="0.3">
@@ -16292,10 +16292,10 @@
         <v>338</v>
       </c>
       <c r="U206" s="2">
-        <v>15.5997</v>
+        <v>14.966699999999999</v>
       </c>
       <c r="V206" s="2">
-        <v>-87.199100000000001</v>
+        <v>-88.025999999999996</v>
       </c>
     </row>
     <row r="207" spans="1:22" x14ac:dyDescent="0.3">
@@ -16360,10 +16360,10 @@
         <v>344</v>
       </c>
       <c r="U207" s="2">
-        <v>15.5997</v>
+        <v>13.3119</v>
       </c>
       <c r="V207" s="2">
-        <v>-87.198899999999995</v>
+        <v>-87.177300000000002</v>
       </c>
     </row>
     <row r="208" spans="1:22" x14ac:dyDescent="0.3">
@@ -16428,10 +16428,10 @@
         <v>308</v>
       </c>
       <c r="U208" s="2">
-        <v>15.5997</v>
+        <v>13.4322</v>
       </c>
       <c r="V208" s="2">
-        <v>-87.198800000000006</v>
+        <v>-86.808099999999996</v>
       </c>
     </row>
     <row r="209" spans="1:22" x14ac:dyDescent="0.3">
@@ -16496,10 +16496,10 @@
         <v>308</v>
       </c>
       <c r="U209" s="2">
-        <v>15.5997</v>
+        <v>13.432700000000001</v>
       </c>
       <c r="V209" s="2">
-        <v>-87.198499999999996</v>
+        <v>-86.807000000000002</v>
       </c>
     </row>
     <row r="210" spans="1:22" x14ac:dyDescent="0.3">
@@ -16564,10 +16564,10 @@
         <v>350</v>
       </c>
       <c r="U210" s="2">
-        <v>15.5999</v>
+        <v>14.0413</v>
       </c>
       <c r="V210" s="2">
-        <v>-87.201999999999998</v>
+        <v>-87.233099999999993</v>
       </c>
     </row>
     <row r="211" spans="1:22" x14ac:dyDescent="0.3">
@@ -16632,10 +16632,10 @@
         <v>308</v>
       </c>
       <c r="U211" s="2">
-        <v>15.5999</v>
+        <v>14.045199999999999</v>
       </c>
       <c r="V211" s="2">
-        <v>-87.199100000000001</v>
+        <v>-87.211200000000005</v>
       </c>
     </row>
     <row r="212" spans="1:22" x14ac:dyDescent="0.3">
@@ -16700,10 +16700,10 @@
         <v>311</v>
       </c>
       <c r="U212" s="2">
-        <v>15.5999</v>
+        <v>14.0457</v>
       </c>
       <c r="V212" s="2">
-        <v>-87.199399999999997</v>
+        <v>-87.2119</v>
       </c>
     </row>
     <row r="213" spans="1:22" x14ac:dyDescent="0.3">
@@ -16768,10 +16768,10 @@
         <v>351</v>
       </c>
       <c r="U213" s="2">
-        <v>15.6</v>
+        <v>14.0466</v>
       </c>
       <c r="V213" s="2">
-        <v>-87.198999999999998</v>
+        <v>-87.219700000000003</v>
       </c>
     </row>
     <row r="214" spans="1:22" x14ac:dyDescent="0.3">
@@ -16836,10 +16836,10 @@
         <v>309</v>
       </c>
       <c r="U214" s="2">
-        <v>15.600300000000001</v>
+        <v>14.053699999999999</v>
       </c>
       <c r="V214" s="2">
-        <v>-87.215100000000007</v>
+        <v>-87.229500000000002</v>
       </c>
     </row>
     <row r="215" spans="1:22" x14ac:dyDescent="0.3">
@@ -16904,10 +16904,10 @@
         <v>352</v>
       </c>
       <c r="U215" s="2">
-        <v>15.6004</v>
+        <v>14.0571</v>
       </c>
       <c r="V215" s="2">
-        <v>-87.2119</v>
+        <v>-87.236999999999995</v>
       </c>
     </row>
     <row r="216" spans="1:22" x14ac:dyDescent="0.3">
@@ -16972,10 +16972,10 @@
         <v>326</v>
       </c>
       <c r="U216" s="2">
-        <v>15.601000000000001</v>
+        <v>14.0632</v>
       </c>
       <c r="V216" s="2">
-        <v>-87.198999999999998</v>
+        <v>-87.220699999999994</v>
       </c>
     </row>
     <row r="217" spans="1:22" x14ac:dyDescent="0.3">
@@ -17040,10 +17040,10 @@
         <v>353</v>
       </c>
       <c r="U217" s="2">
-        <v>15.601100000000001</v>
+        <v>14.063599999999999</v>
       </c>
       <c r="V217" s="2">
-        <v>-87.199600000000004</v>
+        <v>-87.209800000000001</v>
       </c>
     </row>
     <row r="218" spans="1:22" x14ac:dyDescent="0.3">
@@ -17108,10 +17108,10 @@
         <v>256</v>
       </c>
       <c r="U218" s="2">
-        <v>15.602</v>
+        <v>14.066800000000001</v>
       </c>
       <c r="V218" s="2">
-        <v>-87.212199999999996</v>
+        <v>-87.179400000000001</v>
       </c>
     </row>
     <row r="219" spans="1:22" x14ac:dyDescent="0.3">
@@ -17176,10 +17176,10 @@
         <v>309</v>
       </c>
       <c r="U219" s="2">
-        <v>15.602499999999999</v>
+        <v>14.077299999999999</v>
       </c>
       <c r="V219" s="2">
-        <v>-87.211600000000004</v>
+        <v>-87.186499999999995</v>
       </c>
     </row>
     <row r="220" spans="1:22" x14ac:dyDescent="0.3">
@@ -17244,10 +17244,10 @@
         <v>309</v>
       </c>
       <c r="U220" s="2">
-        <v>15.6463</v>
+        <v>14.0885</v>
       </c>
       <c r="V220" s="2">
-        <v>-87.036000000000001</v>
+        <v>-87.182599999999994</v>
       </c>
     </row>
     <row r="221" spans="1:22" x14ac:dyDescent="0.3">
@@ -17312,10 +17312,10 @@
         <v>354</v>
       </c>
       <c r="U221" s="2">
-        <v>15.6639</v>
+        <v>14.0983</v>
       </c>
       <c r="V221" s="2">
-        <v>-87.045299999999997</v>
+        <v>-87.163600000000002</v>
       </c>
     </row>
     <row r="222" spans="1:22" x14ac:dyDescent="0.3">
@@ -17380,10 +17380,10 @@
         <v>308</v>
       </c>
       <c r="U222" s="2">
-        <v>15.7628</v>
+        <v>14.1006</v>
       </c>
       <c r="V222" s="2">
-        <v>-87.479900000000001</v>
+        <v>-87.209800000000001</v>
       </c>
     </row>
     <row r="223" spans="1:22" x14ac:dyDescent="0.3">
@@ -17448,10 +17448,10 @@
         <v>355</v>
       </c>
       <c r="U223" s="2">
-        <v>15.7629</v>
+        <v>14.1015</v>
       </c>
       <c r="V223" s="2">
-        <v>-87.477099999999993</v>
+        <v>-87.207899999999995</v>
       </c>
     </row>
     <row r="224" spans="1:22" x14ac:dyDescent="0.3">
@@ -17516,10 +17516,10 @@
         <v>309</v>
       </c>
       <c r="U224" s="2">
-        <v>15.7629</v>
+        <v>14.102</v>
       </c>
       <c r="V224" s="2">
-        <v>-87.476699999999994</v>
+        <v>-87.185299999999998</v>
       </c>
     </row>
     <row r="225" spans="1:22" x14ac:dyDescent="0.3">
@@ -17584,10 +17584,10 @@
         <v>308</v>
       </c>
       <c r="U225" s="2">
-        <v>15.7631</v>
+        <v>14.1028</v>
       </c>
       <c r="V225" s="2">
-        <v>-87.476299999999995</v>
+        <v>-87.178700000000006</v>
       </c>
     </row>
     <row r="226" spans="1:22" x14ac:dyDescent="0.3">
@@ -17652,10 +17652,10 @@
         <v>311</v>
       </c>
       <c r="U226" s="2">
-        <v>15.763199999999999</v>
+        <v>14.1046</v>
       </c>
       <c r="V226" s="2">
-        <v>-87.476100000000002</v>
+        <v>-87.205500000000001</v>
       </c>
     </row>
     <row r="227" spans="1:22" x14ac:dyDescent="0.3">
@@ -17720,10 +17720,10 @@
         <v>356</v>
       </c>
       <c r="U227" s="2">
-        <v>15.7651</v>
+        <v>14.1052</v>
       </c>
       <c r="V227" s="2">
-        <v>-87.480400000000003</v>
+        <v>-87.154700000000005</v>
       </c>
     </row>
     <row r="228" spans="1:22" x14ac:dyDescent="0.3">
@@ -17788,10 +17788,10 @@
         <v>256</v>
       </c>
       <c r="U228" s="2">
-        <v>15.766500000000001</v>
+        <v>14.1066</v>
       </c>
       <c r="V228" s="2">
-        <v>-87.48</v>
+        <v>-87.221199999999996</v>
       </c>
     </row>
     <row r="229" spans="1:22" x14ac:dyDescent="0.3">
@@ -17856,10 +17856,10 @@
         <v>357</v>
       </c>
       <c r="U229" s="2">
-        <v>15.767799999999999</v>
+        <v>14.1357</v>
       </c>
       <c r="V229" s="2">
-        <v>-87.480900000000005</v>
+        <v>-87.160799999999995</v>
       </c>
     </row>
     <row r="230" spans="1:22" x14ac:dyDescent="0.3">
@@ -17924,10 +17924,10 @@
         <v>308</v>
       </c>
       <c r="U230" s="2">
-        <v>15.7722</v>
+        <v>14.5405</v>
       </c>
       <c r="V230" s="2">
-        <v>-87.470399999999998</v>
+        <v>-86.830399999999997</v>
       </c>
     </row>
     <row r="231" spans="1:22" x14ac:dyDescent="0.3">
@@ -17992,10 +17992,10 @@
         <v>358</v>
       </c>
       <c r="U231" s="2">
-        <v>15.773400000000001</v>
+        <v>14.552199999999999</v>
       </c>
       <c r="V231" s="2">
-        <v>-87.448700000000002</v>
+        <v>-86.828000000000003</v>
       </c>
     </row>
     <row r="232" spans="1:22" x14ac:dyDescent="0.3">
@@ -18060,10 +18060,10 @@
         <v>359</v>
       </c>
       <c r="U232" s="2">
-        <v>15.7738</v>
+        <v>14.553000000000001</v>
       </c>
       <c r="V232" s="2">
-        <v>-87.475499999999997</v>
+        <v>-86.8279</v>
       </c>
     </row>
     <row r="233" spans="1:22" x14ac:dyDescent="0.3">
@@ -18128,10 +18128,10 @@
         <v>365</v>
       </c>
       <c r="U233" s="2">
-        <v>15.7738</v>
+        <v>14.011799999999999</v>
       </c>
       <c r="V233" s="2">
-        <v>-87.475399999999993</v>
+        <v>-87.013099999999994</v>
       </c>
     </row>
     <row r="234" spans="1:22" x14ac:dyDescent="0.3">
@@ -18196,10 +18196,10 @@
         <v>366</v>
       </c>
       <c r="U234" s="2">
-        <v>15.7738</v>
+        <v>14.1625</v>
       </c>
       <c r="V234" s="2">
-        <v>-87.475300000000004</v>
+        <v>-87.044300000000007</v>
       </c>
     </row>
     <row r="235" spans="1:22" x14ac:dyDescent="0.3">
@@ -18264,10 +18264,10 @@
         <v>308</v>
       </c>
       <c r="U235" s="2">
-        <v>15.774100000000001</v>
+        <v>14.485300000000001</v>
       </c>
       <c r="V235" s="2">
-        <v>-87.464399999999998</v>
+        <v>-87.982699999999994</v>
       </c>
     </row>
     <row r="236" spans="1:22" x14ac:dyDescent="0.3">
@@ -18332,10 +18332,10 @@
         <v>308</v>
       </c>
       <c r="U236" s="2">
-        <v>15.7744</v>
+        <v>14.4856</v>
       </c>
       <c r="V236" s="2">
-        <v>-87.446799999999996</v>
+        <v>-87.982100000000003</v>
       </c>
     </row>
     <row r="237" spans="1:22" x14ac:dyDescent="0.3">
@@ -18400,10 +18400,10 @@
         <v>374</v>
       </c>
       <c r="U237" s="2">
-        <v>15.774699999999999</v>
+        <v>14.485900000000001</v>
       </c>
       <c r="V237" s="2">
-        <v>-87.473600000000005</v>
+        <v>-87.980999999999995</v>
       </c>
     </row>
     <row r="238" spans="1:22" x14ac:dyDescent="0.3">
@@ -18468,10 +18468,10 @@
         <v>375</v>
       </c>
       <c r="U238" s="2">
-        <v>15.775399999999999</v>
+        <v>16.314299999999999</v>
       </c>
       <c r="V238" s="2">
-        <v>-87.444699999999997</v>
+        <v>-86.538499999999999</v>
       </c>
     </row>
     <row r="239" spans="1:22" x14ac:dyDescent="0.3">
@@ -18536,10 +18536,10 @@
         <v>376</v>
       </c>
       <c r="U239" s="2">
-        <v>15.775600000000001</v>
+        <v>16.095099999999999</v>
       </c>
       <c r="V239" s="2">
-        <v>-87.473799999999997</v>
+        <v>-86.892899999999997</v>
       </c>
     </row>
     <row r="240" spans="1:22" x14ac:dyDescent="0.3">
@@ -18604,10 +18604,10 @@
         <v>382</v>
       </c>
       <c r="U240" s="2">
-        <v>15.7789</v>
+        <v>14.246</v>
       </c>
       <c r="V240" s="2">
-        <v>-87.464799999999997</v>
+        <v>-87.8994</v>
       </c>
     </row>
     <row r="241" spans="1:22" x14ac:dyDescent="0.3">
@@ -18672,10 +18672,10 @@
         <v>383</v>
       </c>
       <c r="U241" s="2">
-        <v>15.7791</v>
+        <v>14.438000000000001</v>
       </c>
       <c r="V241" s="2">
-        <v>-87.451700000000002</v>
+        <v>-89.182100000000005</v>
       </c>
     </row>
     <row r="242" spans="1:22" x14ac:dyDescent="0.3">
@@ -18740,10 +18740,10 @@
         <v>389</v>
       </c>
       <c r="U242" s="2">
-        <v>15.7791</v>
+        <v>13.5337</v>
       </c>
       <c r="V242" s="2">
-        <v>-87.451700000000002</v>
+        <v>-87.496300000000005</v>
       </c>
     </row>
     <row r="243" spans="1:22" x14ac:dyDescent="0.3">
@@ -18808,10 +18808,10 @@
         <v>311</v>
       </c>
       <c r="U243" s="2">
-        <v>15.7791</v>
+        <v>13.4329</v>
       </c>
       <c r="V243" s="2">
-        <v>-87.451700000000002</v>
+        <v>-87.450699999999998</v>
       </c>
     </row>
     <row r="244" spans="1:22" x14ac:dyDescent="0.3">
@@ -18876,10 +18876,10 @@
         <v>394</v>
       </c>
       <c r="U244" s="2">
-        <v>15.779199999999999</v>
+        <v>15.4025</v>
       </c>
       <c r="V244" s="2">
-        <v>-87.464799999999997</v>
+        <v>-87.796800000000005</v>
       </c>
     </row>
     <row r="245" spans="1:22" x14ac:dyDescent="0.3">
@@ -18944,10 +18944,10 @@
         <v>394</v>
       </c>
       <c r="U245" s="2">
-        <v>15.780099999999999</v>
+        <v>15.4025</v>
       </c>
       <c r="V245" s="2">
-        <v>-87.457400000000007</v>
+        <v>-87.796800000000005</v>
       </c>
     </row>
     <row r="246" spans="1:22" x14ac:dyDescent="0.3">
@@ -19012,10 +19012,10 @@
         <v>308</v>
       </c>
       <c r="U246" s="2">
-        <v>15.780099999999999</v>
+        <v>15.402900000000001</v>
       </c>
       <c r="V246" s="2">
-        <v>-87.457300000000004</v>
+        <v>-87.806899999999999</v>
       </c>
     </row>
     <row r="247" spans="1:22" x14ac:dyDescent="0.3">
@@ -19080,10 +19080,10 @@
         <v>308</v>
       </c>
       <c r="U247" s="2">
-        <v>15.780099999999999</v>
+        <v>15.402900000000001</v>
       </c>
       <c r="V247" s="2">
-        <v>-87.457300000000004</v>
+        <v>-87.806899999999999</v>
       </c>
     </row>
     <row r="248" spans="1:22" x14ac:dyDescent="0.3">
@@ -19148,10 +19148,10 @@
         <v>397</v>
       </c>
       <c r="U248" s="2">
-        <v>15.780099999999999</v>
+        <v>15.3802</v>
       </c>
       <c r="V248" s="2">
-        <v>-87.4572</v>
+        <v>-87.808700000000002</v>
       </c>
     </row>
     <row r="249" spans="1:22" x14ac:dyDescent="0.3">
@@ -19216,10 +19216,10 @@
         <v>400</v>
       </c>
       <c r="U249" s="2">
-        <v>15.7803</v>
+        <v>15.3644</v>
       </c>
       <c r="V249" s="2">
-        <v>-87.456800000000001</v>
+        <v>-87.791200000000003</v>
       </c>
     </row>
     <row r="250" spans="1:22" x14ac:dyDescent="0.3">
@@ -19284,10 +19284,10 @@
         <v>403</v>
       </c>
       <c r="U250" s="2">
-        <v>15.7803</v>
+        <v>15.420199999999999</v>
       </c>
       <c r="V250" s="2">
-        <v>-87.456699999999998</v>
+        <v>-87.786000000000001</v>
       </c>
     </row>
     <row r="251" spans="1:22" x14ac:dyDescent="0.3">
@@ -19352,10 +19352,10 @@
         <v>409</v>
       </c>
       <c r="U251" s="2">
-        <v>15.7803</v>
+        <v>15.320600000000001</v>
       </c>
       <c r="V251" s="2">
-        <v>-87.476900000000001</v>
+        <v>-87.600700000000003</v>
       </c>
     </row>
     <row r="252" spans="1:22" x14ac:dyDescent="0.3">
@@ -19420,10 +19420,10 @@
         <v>410</v>
       </c>
       <c r="U252" s="2">
-        <v>15.7804</v>
+        <v>15.321099999999999</v>
       </c>
       <c r="V252" s="2">
-        <v>-87.451800000000006</v>
+        <v>-87.5989</v>
       </c>
     </row>
     <row r="253" spans="1:22" x14ac:dyDescent="0.3">
@@ -19488,10 +19488,10 @@
         <v>411</v>
       </c>
       <c r="U253" s="2">
-        <v>15.7804</v>
+        <v>14.106299999999999</v>
       </c>
       <c r="V253" s="2">
-        <v>-87.456999999999994</v>
+        <v>-87.218900000000005</v>
       </c>
     </row>
     <row r="254" spans="1:22" x14ac:dyDescent="0.3">
@@ -19556,10 +19556,10 @@
         <v>412</v>
       </c>
       <c r="U254" s="2">
-        <v>15.7804</v>
+        <v>16.0976</v>
       </c>
       <c r="V254" s="2">
-        <v>-87.453800000000001</v>
+        <v>-86.896100000000004</v>
       </c>
     </row>
     <row r="255" spans="1:22" x14ac:dyDescent="0.3">
@@ -19624,10 +19624,10 @@
         <v>413</v>
       </c>
       <c r="U255" s="2">
-        <v>15.7805</v>
+        <v>14.5892</v>
       </c>
       <c r="V255" s="2">
-        <v>-87.456800000000001</v>
+        <v>-88.582599999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-28-2020 21-48-54
</commit_message>
<xml_diff>
--- a/datacovidhn/ALIMENTACION_HN.xlsx
+++ b/datacovidhn/ALIMENTACION_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="8_{2E7B08DD-615A-4A26-9C8E-D4330F5D4097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E45FD08E-DFDF-41BE-AA89-E604E4FCC90A}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="8_{2E7B08DD-615A-4A26-9C8E-D4330F5D4097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F6433AE5-3CEB-4ECD-A184-4A5696E6CCA0}"/>
   <bookViews>
     <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ALIMENTACION" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ALIMENTACION!$A$1:$V$256</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ALIMENTACION!$A$1:$V$255</definedName>
     <definedName name="_xlnm.Database">ALIMENTACION!$A$1:$T$255</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3847" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3832" uniqueCount="419">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -1930,8 +1930,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3102A056-5222-4234-BA9B-734A45734C30}" name="ALIMENTACION_HN" displayName="ALIMENTACION_HN" ref="A1:V256" totalsRowShown="0" headerRowDxfId="22">
-  <autoFilter ref="A1:V256" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3102A056-5222-4234-BA9B-734A45734C30}" name="ALIMENTACION_HN" displayName="ALIMENTACION_HN" ref="A1:V255" totalsRowShown="0" headerRowDxfId="22">
+  <autoFilter ref="A1:V255" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{72EFC8A3-7F7E-43ED-A5A6-542387FEE48F}" name="OBJECTID_1" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{E5F0AA7C-EAE9-4EBF-8A11-FABC8E4AD95A}" name="Pais_cod3" dataDxfId="20"/>
@@ -2257,11 +2257,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V256"/>
+  <dimension ref="A1:V255"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B256" sqref="B256"/>
+      <pane ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B257" sqref="B257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -19630,74 +19630,6 @@
         <v>-88.582599999999999</v>
       </c>
     </row>
-    <row r="256" spans="1:22">
-      <c r="A256" s="1">
-        <v>28207</v>
-      </c>
-      <c r="B256" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C256" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D256" s="1">
-        <v>3</v>
-      </c>
-      <c r="E256" s="1">
-        <v>3</v>
-      </c>
-      <c r="F256" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G256" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H256" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I256" s="1">
-        <v>18</v>
-      </c>
-      <c r="J256" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K256" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L256" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M256" s="1">
-        <v>1</v>
-      </c>
-      <c r="N256" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O256" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P256" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q256" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="R256" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S256" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="T256" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="U256" s="2">
-        <v>14.591900000000001</v>
-      </c>
-      <c r="V256" s="2">
-        <v>-87.834199999999996</v>
-      </c>
-    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T255">
     <sortCondition ref="R2:R255"/>

</xml_diff>